<commit_message>
added excel index to project and added some fields
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/221111_Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/221111_Booklet_FK_Lagerlogistik.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erds001\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5FB2F2-E9D5-4C1E-849E-68EE615573E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1BBEEC-16FE-4D31-A6EB-D309BB544987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="972" yWindow="0" windowWidth="23016" windowHeight="25200" firstSheet="1" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="348">
   <si>
     <t>ItemID</t>
   </si>
@@ -1073,6 +1073,30 @@
   </si>
   <si>
     <t>SK34F04_Karte.png</t>
+  </si>
+  <si>
+    <t>AssessmentType</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Disclaimer</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>EscoOccupationId</t>
+  </si>
+  <si>
+    <t>EscoSkills</t>
+  </si>
+  <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Title</t>
   </si>
 </sst>
 </file>
@@ -1308,8 +1332,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
     <dxf>
@@ -1787,9 +1811,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}" name="Tabelle5" displayName="Tabelle5" ref="A1:BB29" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="A1:BB29" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}"/>
-  <tableColumns count="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}" name="Tabelle5" displayName="Tabelle5" ref="A1:BJ29" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A1:BJ29" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}"/>
+  <tableColumns count="62">
     <tableColumn id="1" xr3:uid="{5027A3BA-AE24-48AB-84F1-2B75CE07B771}" name="ItemID"/>
     <tableColumn id="67" xr3:uid="{CBBAA5D6-4174-439A-84DE-FDF2F323CBA9}" name="ReliantOn"/>
     <tableColumn id="3" xr3:uid="{F25AA728-9937-4EC2-9415-03B9BFCFFD36}" name="ItemTyp"/>
@@ -1844,6 +1868,14 @@
     <tableColumn id="73" xr3:uid="{915510BC-5087-4B95-97C8-0143692AE4B0}" name="ProfessionalEscoSkills"/>
     <tableColumn id="75" xr3:uid="{A503BA23-49C3-4C2C-8767-9C35130C28F9}" name="ProfessionalEscoID"/>
     <tableColumn id="65" xr3:uid="{7DF0DE50-5D2C-4DC5-BD98-3D1E5CE5A98E}" name="ForcedChoice"/>
+    <tableColumn id="2" xr3:uid="{4DF2333F-1CF9-45FA-9B10-360A37A1F5E5}" name="AssessmentType"/>
+    <tableColumn id="26" xr3:uid="{14A8CFF7-3400-48DB-A157-F78870D95DFE}" name="Description"/>
+    <tableColumn id="27" xr3:uid="{AA40A9E5-98C7-40FB-9840-AF26971B2CC8}" name="Disclaimer"/>
+    <tableColumn id="28" xr3:uid="{6BC0E4F4-6519-4229-AA93-D62F59406FB7}" name="Duration"/>
+    <tableColumn id="29" xr3:uid="{847AA692-C832-4384-B165-9C5BAD165D97}" name="EscoOccupationId"/>
+    <tableColumn id="34" xr3:uid="{D0177EBA-C7CA-455E-97F8-81D6060CE6AA}" name="EscoSkills"/>
+    <tableColumn id="35" xr3:uid="{6B06B292-43A5-4F34-9035-3EA804E0EE0F}" name="Publisher"/>
+    <tableColumn id="36" xr3:uid="{1835239A-CDDA-4ACD-9EB0-31FD39EA744E}" name="Title"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1865,7 +1897,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2161,15 +2193,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
-  <dimension ref="A1:BB29"/>
+  <dimension ref="A1:BJ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
+      <selection activeCell="BJ2" sqref="BJ2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:54" ht="39.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:62" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2332,8 +2364,32 @@
       <c r="BB1" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC1" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="BF1" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="BH1" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="BI1" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="BJ1" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2382,8 +2438,11 @@
       <c r="AU2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -2435,8 +2494,11 @@
       <c r="AU3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>77</v>
       </c>
@@ -2485,8 +2547,11 @@
       <c r="AU4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -2538,8 +2603,11 @@
       <c r="AU5" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -2591,8 +2659,11 @@
       <c r="AU6" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>102</v>
       </c>
@@ -2644,8 +2715,11 @@
       <c r="AU7" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>109</v>
       </c>
@@ -2695,8 +2769,11 @@
       <c r="AU8" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>112</v>
       </c>
@@ -2748,8 +2825,11 @@
       <c r="AU9" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>120</v>
       </c>
@@ -2810,8 +2890,11 @@
       <c r="AU10" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>131</v>
       </c>
@@ -2860,8 +2943,11 @@
       <c r="AU11" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -2910,8 +2996,11 @@
       <c r="AU12" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -2960,8 +3049,11 @@
       <c r="AU13" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="14" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>148</v>
       </c>
@@ -3010,8 +3102,11 @@
       <c r="AU14" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="15" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -3060,8 +3155,11 @@
       <c r="AU15" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="16" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="BC15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>164</v>
       </c>
@@ -3113,8 +3211,11 @@
       <c r="AU16" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="17" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>171</v>
       </c>
@@ -3163,8 +3264,11 @@
       <c r="AU17" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="18" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>175</v>
       </c>
@@ -3213,8 +3317,11 @@
       <c r="AU18" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="19" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>183</v>
       </c>
@@ -3263,8 +3370,11 @@
       <c r="AU19" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="20" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>186</v>
       </c>
@@ -3313,8 +3423,11 @@
       <c r="AU20" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="21" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>194</v>
       </c>
@@ -3366,8 +3479,11 @@
       <c r="AU21" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="22" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>202</v>
       </c>
@@ -3419,8 +3535,11 @@
       <c r="AU22" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="23" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>209</v>
       </c>
@@ -3472,8 +3591,11 @@
       <c r="AU23" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="24" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>216</v>
       </c>
@@ -3525,8 +3647,11 @@
       <c r="AU24" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="25" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>223</v>
       </c>
@@ -3578,8 +3703,11 @@
       <c r="AU25" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="26" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>231</v>
       </c>
@@ -3628,8 +3756,11 @@
       <c r="AU26" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="27" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>239</v>
       </c>
@@ -3681,8 +3812,11 @@
       <c r="AU27" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="28" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>246</v>
       </c>
@@ -3734,8 +3868,11 @@
       <c r="AU28" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="29" spans="1:47" x14ac:dyDescent="0.25">
+      <c r="BC28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>253</v>
       </c>
@@ -3786,6 +3923,9 @@
       </c>
       <c r="AU29" t="s">
         <v>259</v>
+      </c>
+      <c r="BC29">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3807,24 +3947,24 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.81640625" customWidth="1"/>
-    <col min="2" max="2" width="21.1796875" customWidth="1"/>
-    <col min="3" max="3" width="37.1796875" customWidth="1"/>
-    <col min="4" max="4" width="32.453125" customWidth="1"/>
+    <col min="1" max="1" width="22.77734375" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" customWidth="1"/>
+    <col min="3" max="3" width="37.21875" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>260</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:7" ht="39" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>261</v>
       </c>
@@ -3844,7 +3984,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="51.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>267</v>
       </c>
@@ -3880,7 +4020,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8" t="s">
@@ -3890,7 +4030,7 @@
       <c r="E5" s="11"/>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:7" ht="17.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8" t="s">
@@ -3931,7 +4071,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="7"/>
     </row>
-    <row r="9" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
@@ -3951,7 +4091,7 @@
       <c r="E10" s="9"/>
       <c r="F10" s="7"/>
     </row>
-    <row r="11" spans="1:7" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>284</v>
       </c>
@@ -3969,7 +4109,7 @@
       </c>
       <c r="F11" s="7"/>
     </row>
-    <row r="12" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
@@ -3979,7 +4119,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:7" ht="23.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">
@@ -3989,7 +4129,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="32.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>289</v>
       </c>
@@ -4017,7 +4157,7 @@
       <c r="E15" s="10"/>
       <c r="F15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>294</v>
       </c>
@@ -4045,7 +4185,7 @@
       <c r="E17" s="8"/>
       <c r="F17" s="7"/>
     </row>
-    <row r="18" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8" t="s">
@@ -4055,7 +4195,7 @@
       <c r="E18" s="8"/>
       <c r="F18" s="7"/>
     </row>
-    <row r="19" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="8"/>
       <c r="C19" s="8" t="s">
@@ -4065,7 +4205,7 @@
       <c r="E19" s="8"/>
       <c r="F19" s="7"/>
     </row>
-    <row r="20" spans="1:6" ht="32.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>300</v>
       </c>
@@ -4085,7 +4225,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9" t="s">
@@ -4095,7 +4235,7 @@
       <c r="E21" s="9"/>
       <c r="F21" s="7"/>
     </row>
-    <row r="22" spans="1:6" ht="23.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="23.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9" t="s">
@@ -4105,7 +4245,7 @@
       <c r="E22" s="9"/>
       <c r="F22" s="7"/>
     </row>
-    <row r="23" spans="1:6" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9" t="s">
@@ -4115,7 +4255,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="7"/>
     </row>
-    <row r="24" spans="1:6" ht="25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>307</v>
       </c>
@@ -4133,7 +4273,7 @@
       </c>
       <c r="F24" s="7"/>
     </row>
-    <row r="25" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8"/>
       <c r="B25" s="8"/>
       <c r="C25" s="8" t="s">
@@ -4143,7 +4283,7 @@
       <c r="E25" s="8"/>
       <c r="F25" s="7"/>
     </row>
-    <row r="26" spans="1:6" ht="20.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="8" t="s">
@@ -4173,8 +4313,8 @@
       <c r="E28" s="8"/>
       <c r="F28" s="7"/>
     </row>
-    <row r="29" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:6" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="123" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="159" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="163" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4193,17 +4333,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100879B58D3C23DCA4AAEF47596CA4D8E48" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee8b9d8723b80ccc4cb578ffd4faacc7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02625a54-df84-4a3b-b049-0bb7e92cde0d" xmlns:ns3="c90f9e10-81f0-426e-b8bb-fc89022b3796" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64b8ed4db9a6e136c161da669116b9cc" ns2:_="" ns3:_="">
     <xsd:import namespace="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
@@ -4412,6 +4541,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4422,23 +4562,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A223085B-57B4-40DB-BC96-92703C914FDC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4457,6 +4580,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fixed a lot of Asscociate shit
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/221111_Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/221111_Booklet_FK_Lagerlogistik.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanaBoscolo\source\repos\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1BBEEC-16FE-4D31-A6EB-D309BB544987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C39CC2-1B97-4548-89DD-B05778DB1DD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="972" yWindow="0" windowWidth="23016" windowHeight="25200" firstSheet="1" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="18300" yWindow="6345" windowWidth="32235" windowHeight="21945" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="354">
   <si>
     <t>ItemID</t>
   </si>
@@ -244,9 +244,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bei der Prüfung einer Lieferung siehst du, dass ein Karton auf der Palette eingerissen ist. Was tust du? </t>
-  </si>
-  <si>
-    <t>Bild</t>
   </si>
   <si>
     <t>Bitte wähle 1 bis 3 Antworten aus.</t>
@@ -983,12 +980,6 @@
     <t xml:space="preserve">G. Vertragsdokumente kontrollieren </t>
   </si>
   <si>
-    <t>SK34B02_Pfuetze_Gabelstapler.jpg</t>
-  </si>
-  <si>
-    <t>SK34B04_Zeichen_Zerbrechlich.JPG</t>
-  </si>
-  <si>
     <t>Kühllager</t>
   </si>
   <si>
@@ -1001,47 +992,6 @@
     <t>Überdachtes Außenlager</t>
   </si>
   <si>
-    <t>SK34E01_Luftpolsterfolie.jpg</t>
-  </si>
-  <si>
-    <t>SK34E01_Folie.jpg</t>
-  </si>
-  <si>
-    <t>SK34E01_Pappkarton.jpg</t>
-  </si>
-  <si>
-    <t>SK34E01_Zeitung.jpg</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1 - 0 - 0 - </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-  </si>
-  <si>
-    <t>SK34E03_Spanngurt.jpg</t>
-  </si>
-  <si>
-    <t>SK34E03_Folie.jpg</t>
-  </si>
-  <si>
-    <t>SK34E03_Spannband.jpg</t>
-  </si>
-  <si>
-    <t>SK34E03_Tape.jpg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kein Bild </t>
-  </si>
-  <si>
     <t>SK34C01_nicht_stapeln.png</t>
   </si>
   <si>
@@ -1060,18 +1010,6 @@
     <t>SK34G03_Vergleichsmatrix.png</t>
   </si>
   <si>
-    <t>SK34B03_Hubwagen_D1.JPG</t>
-  </si>
-  <si>
-    <t>SK34B03_Hubwagen_D2.JPG</t>
-  </si>
-  <si>
-    <t>SK34B03_Hubwagen_D3.JPG</t>
-  </si>
-  <si>
-    <t>SK34B03_Hubwagen_A1.JPG</t>
-  </si>
-  <si>
     <t>SK34F04_Karte.png</t>
   </si>
   <si>
@@ -1097,13 +1035,82 @@
   </si>
   <si>
     <t>Title</t>
+  </si>
+  <si>
+    <t>CHOICE_QP</t>
+  </si>
+  <si>
+    <t>CHOICE_AP</t>
+  </si>
+  <si>
+    <t>IMAGEMAP</t>
+  </si>
+  <si>
+    <t>SK34A02_Karton_eingerissen.png</t>
+  </si>
+  <si>
+    <t>SK34B01_Sicherheitshinweis_Schuhe</t>
+  </si>
+  <si>
+    <t>SK34B02_Pfuetze_Gabelstapler.png</t>
+  </si>
+  <si>
+    <t>SK34B04_Zeichen_Zerbrechlich.png</t>
+  </si>
+  <si>
+    <t>SK34C03_Regaltraeger_Zeichnung.png</t>
+  </si>
+  <si>
+    <t>SK34D03_Regalbezeichnung.png</t>
+  </si>
+  <si>
+    <t>SK34B03_Hubwagen_D1.png</t>
+  </si>
+  <si>
+    <t>SK34B03_Hubwagen_A1.png</t>
+  </si>
+  <si>
+    <t>SK34B03_Hubwagen_D2.png</t>
+  </si>
+  <si>
+    <t>SK34B03_Hubwagen_D3.png</t>
+  </si>
+  <si>
+    <t>SK34E01_Luftpolsterfolie.png</t>
+  </si>
+  <si>
+    <t>SK34E01_Folie.png</t>
+  </si>
+  <si>
+    <t>SK34E01_Pappkarton.png</t>
+  </si>
+  <si>
+    <t>SK34E01_Zeitung.png</t>
+  </si>
+  <si>
+    <t>SK34E03_Spanngurt.png</t>
+  </si>
+  <si>
+    <t>SK34E03_Folie.png</t>
+  </si>
+  <si>
+    <t>SK34E03_Spannband.png</t>
+  </si>
+  <si>
+    <t>SK34E03_Tape.png</t>
+  </si>
+  <si>
+    <t>LIMIT</t>
+  </si>
+  <si>
+    <t>CourseId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -1168,12 +1175,6 @@
     <font>
       <sz val="10"/>
       <color theme="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF92D050"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1286,7 +1287,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1300,7 +1301,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1328,8 +1328,16 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1811,9 +1819,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}" name="Tabelle5" displayName="Tabelle5" ref="A1:BJ29" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
-  <autoFilter ref="A1:BJ29" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}"/>
-  <tableColumns count="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}" name="Tabelle5" displayName="Tabelle5" ref="A1:BL29" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="A1:BL29" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}"/>
+  <tableColumns count="64">
     <tableColumn id="1" xr3:uid="{5027A3BA-AE24-48AB-84F1-2B75CE07B771}" name="ItemID"/>
     <tableColumn id="67" xr3:uid="{CBBAA5D6-4174-439A-84DE-FDF2F323CBA9}" name="ReliantOn"/>
     <tableColumn id="3" xr3:uid="{F25AA728-9937-4EC2-9415-03B9BFCFFD36}" name="ItemTyp"/>
@@ -1876,6 +1884,8 @@
     <tableColumn id="34" xr3:uid="{D0177EBA-C7CA-455E-97F8-81D6060CE6AA}" name="EscoSkills"/>
     <tableColumn id="35" xr3:uid="{6B06B292-43A5-4F34-9035-3EA804E0EE0F}" name="Publisher"/>
     <tableColumn id="36" xr3:uid="{1835239A-CDDA-4ACD-9EB0-31FD39EA744E}" name="Title"/>
+    <tableColumn id="37" xr3:uid="{90C2C4A1-CF0D-4B56-8B42-919DD531C4C0}" name="LIMIT"/>
+    <tableColumn id="38" xr3:uid="{179223B5-3B0E-4CBE-B1C9-0C2EA9F0C960}" name="CourseId"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2193,15 +2203,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
-  <dimension ref="A1:BJ29"/>
+  <dimension ref="A1:BL29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="BJ2" sqref="BJ2"/>
+    <sheetView tabSelected="1" topLeftCell="AU1" workbookViewId="0">
+      <selection activeCell="BM34" sqref="BM34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" customWidth="1"/>
+    <col min="46" max="46" width="38.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:64" ht="39" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2365,31 +2381,37 @@
         <v>53</v>
       </c>
       <c r="BC1" s="2" t="s">
-        <v>340</v>
+        <v>323</v>
       </c>
       <c r="BD1" s="2" t="s">
-        <v>341</v>
+        <v>324</v>
       </c>
       <c r="BE1" s="2" t="s">
-        <v>342</v>
+        <v>325</v>
       </c>
       <c r="BF1" s="2" t="s">
-        <v>343</v>
+        <v>326</v>
       </c>
       <c r="BG1" s="2" t="s">
-        <v>344</v>
+        <v>327</v>
       </c>
       <c r="BH1" s="2" t="s">
-        <v>345</v>
+        <v>328</v>
       </c>
       <c r="BI1" s="2" t="s">
-        <v>346</v>
+        <v>329</v>
       </c>
       <c r="BJ1" s="2" t="s">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
+        <v>330</v>
+      </c>
+      <c r="BK1" s="22" t="s">
+        <v>352</v>
+      </c>
+      <c r="BL1" s="22" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2399,6 +2421,7 @@
       <c r="D2" t="s">
         <v>56</v>
       </c>
+      <c r="F2" s="16"/>
       <c r="J2" t="s">
         <v>57</v>
       </c>
@@ -2408,19 +2431,21 @@
       <c r="N2">
         <v>4</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="U2" t="s">
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="21" t="s">
         <v>62</v>
       </c>
       <c r="AK2">
@@ -2441,22 +2466,28 @@
       <c r="BC2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK2">
+        <v>3</v>
+      </c>
+      <c r="BL2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>67</v>
+        <v>331</v>
       </c>
       <c r="D3" t="s">
         <v>68</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="J3" t="s">
         <v>69</v>
-      </c>
-      <c r="J3" t="s">
-        <v>70</v>
       </c>
       <c r="L3">
         <v>4</v>
@@ -2464,20 +2495,22 @@
       <c r="N3">
         <v>3</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="P3" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" s="19"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="21" t="s">
         <v>74</v>
-      </c>
-      <c r="U3" t="s">
-        <v>75</v>
       </c>
       <c r="AK3">
         <v>1</v>
@@ -2492,24 +2525,31 @@
         <v>64</v>
       </c>
       <c r="AU3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="BC3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK3">
+        <v>3</v>
+      </c>
+      <c r="BL3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
         <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="F4" s="16"/>
       <c r="J4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L4">
         <v>4</v>
@@ -2517,20 +2557,22 @@
       <c r="N4">
         <v>3</v>
       </c>
-      <c r="O4" t="s">
+      <c r="O4" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="P4" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="21" t="s">
         <v>82</v>
-      </c>
-      <c r="U4" t="s">
-        <v>83</v>
       </c>
       <c r="AK4">
         <v>1</v>
@@ -2545,27 +2587,31 @@
         <v>64</v>
       </c>
       <c r="AU4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="BC4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK4" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C5" t="s">
         <v>67</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>328</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="F5" s="18"/>
       <c r="J5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L5">
         <v>4</v>
@@ -2573,20 +2619,22 @@
       <c r="N5">
         <v>3</v>
       </c>
-      <c r="O5" t="s">
+      <c r="O5" s="19" t="s">
+        <v>86</v>
+      </c>
+      <c r="P5" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" s="19"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="21" t="s">
         <v>90</v>
-      </c>
-      <c r="U5" t="s">
-        <v>91</v>
       </c>
       <c r="AK5">
         <v>1</v>
@@ -2601,27 +2649,33 @@
         <v>64</v>
       </c>
       <c r="AU5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="BC5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK5" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" t="s">
+        <v>331</v>
+      </c>
+      <c r="D6" t="s">
         <v>93</v>
       </c>
-      <c r="C6" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>94</v>
-      </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="17" t="s">
+        <v>335</v>
+      </c>
+      <c r="J6" t="s">
         <v>69</v>
-      </c>
-      <c r="J6" t="s">
-        <v>70</v>
       </c>
       <c r="L6">
         <v>4</v>
@@ -2629,20 +2683,22 @@
       <c r="N6">
         <v>3</v>
       </c>
-      <c r="O6" t="s">
+      <c r="O6" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="P6" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" s="19"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="21" t="s">
         <v>98</v>
-      </c>
-      <c r="U6" t="s">
-        <v>99</v>
       </c>
       <c r="AK6">
         <v>1</v>
@@ -2654,30 +2710,36 @@
         <v>51312</v>
       </c>
       <c r="AT6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AU6" t="s">
         <v>100</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>101</v>
       </c>
       <c r="BC6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK6" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" t="s">
+        <v>331</v>
+      </c>
+      <c r="D7" t="s">
         <v>102</v>
       </c>
-      <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" t="s">
-        <v>103</v>
-      </c>
       <c r="F7" s="17" t="s">
-        <v>313</v>
+        <v>336</v>
       </c>
       <c r="J7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L7">
         <v>4</v>
@@ -2685,20 +2747,22 @@
       <c r="N7">
         <v>3</v>
       </c>
-      <c r="O7" t="s">
+      <c r="O7" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="P7" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="R7" t="s">
-        <v>107</v>
-      </c>
-      <c r="U7" t="s">
-        <v>83</v>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="21" t="s">
+        <v>82</v>
       </c>
       <c r="AK7">
         <v>1</v>
@@ -2710,27 +2774,34 @@
         <v>51312</v>
       </c>
       <c r="AT7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AU7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="BC7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK7" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" t="s">
+        <v>332</v>
+      </c>
+      <c r="D8" t="s">
         <v>109</v>
       </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" t="s">
-        <v>110</v>
-      </c>
+      <c r="F8" s="16"/>
       <c r="J8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L8">
         <v>4</v>
@@ -2738,21 +2809,22 @@
       <c r="N8">
         <v>3</v>
       </c>
-      <c r="O8" s="18" t="s">
-        <v>335</v>
-      </c>
-      <c r="P8" s="18" t="s">
-        <v>338</v>
-      </c>
-      <c r="Q8" s="18" t="s">
-        <v>336</v>
-      </c>
-      <c r="R8" s="18" t="s">
-        <v>337</v>
-      </c>
-      <c r="S8" s="18"/>
-      <c r="U8" t="s">
-        <v>91</v>
+      <c r="O8" s="20" t="s">
+        <v>340</v>
+      </c>
+      <c r="P8" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="Q8" s="20" t="s">
+        <v>342</v>
+      </c>
+      <c r="R8" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="S8" s="19"/>
+      <c r="T8" s="19"/>
+      <c r="U8" s="21" t="s">
+        <v>90</v>
       </c>
       <c r="AK8">
         <v>1</v>
@@ -2764,30 +2836,36 @@
         <v>51312</v>
       </c>
       <c r="AT8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AU8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="BC8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK8" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" t="s">
+        <v>331</v>
+      </c>
+      <c r="D9" t="s">
         <v>112</v>
       </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" t="s">
-        <v>113</v>
-      </c>
       <c r="F9" s="17" t="s">
-        <v>314</v>
+        <v>337</v>
       </c>
       <c r="J9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L9">
         <v>4</v>
@@ -2795,20 +2873,22 @@
       <c r="N9">
         <v>3</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="P9" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" s="19" t="s">
         <v>115</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" s="19"/>
+      <c r="T9" s="19"/>
+      <c r="U9" s="21" t="s">
         <v>117</v>
-      </c>
-      <c r="U9" t="s">
-        <v>118</v>
       </c>
       <c r="AK9">
         <v>1</v>
@@ -2820,27 +2900,34 @@
         <v>51312</v>
       </c>
       <c r="AT9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AU9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="BC9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK9" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" t="s">
         <v>120</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>121</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" s="16"/>
+      <c r="J10" t="s">
         <v>122</v>
-      </c>
-      <c r="J10" t="s">
-        <v>123</v>
       </c>
       <c r="L10">
         <v>4</v>
@@ -2848,32 +2935,34 @@
       <c r="N10">
         <v>4</v>
       </c>
-      <c r="O10" s="17" t="s">
-        <v>329</v>
-      </c>
-      <c r="P10" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="Q10" s="17" t="s">
-        <v>331</v>
-      </c>
-      <c r="R10" s="17" t="s">
-        <v>332</v>
-      </c>
-      <c r="U10" t="s">
+      <c r="O10" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="P10" s="19" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q10" s="19" t="s">
+        <v>318</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="S10" s="19"/>
+      <c r="T10" s="19"/>
+      <c r="U10" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA10" t="s">
         <v>124</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>125</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>126</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>127</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>128</v>
       </c>
       <c r="AK10">
         <v>1</v>
@@ -2885,27 +2974,34 @@
         <v>51312</v>
       </c>
       <c r="AT10" t="s">
+        <v>128</v>
+      </c>
+      <c r="AU10" t="s">
         <v>129</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>130</v>
       </c>
       <c r="BC10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK10" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C11" t="s">
         <v>67</v>
       </c>
       <c r="D11" t="s">
-        <v>132</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="F11" s="16"/>
       <c r="J11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L11">
         <v>4</v>
@@ -2913,20 +3009,22 @@
       <c r="N11">
         <v>3</v>
       </c>
-      <c r="O11" s="17" t="s">
+      <c r="O11" s="19" t="s">
+        <v>312</v>
+      </c>
+      <c r="P11" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q11" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="R11" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="P11" s="17" t="s">
-        <v>316</v>
-      </c>
-      <c r="Q11" s="17" t="s">
-        <v>317</v>
-      </c>
-      <c r="R11" s="17" t="s">
-        <v>318</v>
-      </c>
-      <c r="U11" t="s">
-        <v>133</v>
+      <c r="S11" s="19"/>
+      <c r="T11" s="19"/>
+      <c r="U11" s="21" t="s">
+        <v>132</v>
       </c>
       <c r="AK11">
         <v>1</v>
@@ -2938,30 +3036,36 @@
         <v>51312</v>
       </c>
       <c r="AT11" t="s">
+        <v>128</v>
+      </c>
+      <c r="AU11" t="s">
         <v>129</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>130</v>
       </c>
       <c r="BC11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK11" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" t="s">
+        <v>331</v>
+      </c>
+      <c r="D12" t="s">
         <v>134</v>
       </c>
-      <c r="C12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" t="s">
-        <v>135</v>
-      </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="17" t="s">
+        <v>338</v>
+      </c>
+      <c r="J12" t="s">
         <v>69</v>
-      </c>
-      <c r="J12" t="s">
-        <v>70</v>
       </c>
       <c r="L12">
         <v>4</v>
@@ -2969,17 +3073,20 @@
       <c r="N12">
         <v>3</v>
       </c>
-      <c r="O12" t="s">
+      <c r="O12" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="P12" s="19" t="s">
         <v>136</v>
       </c>
-      <c r="P12" t="s">
+      <c r="Q12" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="Q12" t="s">
-        <v>138</v>
-      </c>
-      <c r="U12" t="s">
-        <v>118</v>
+      <c r="R12" s="19"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="19"/>
+      <c r="U12" s="21" t="s">
+        <v>117</v>
       </c>
       <c r="AK12">
         <v>1</v>
@@ -2991,27 +3098,34 @@
         <v>51312</v>
       </c>
       <c r="AT12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AU12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BC12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK12" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C13" t="s">
         <v>67</v>
       </c>
       <c r="D13" t="s">
-        <v>141</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F13" s="16"/>
       <c r="J13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L13">
         <v>4</v>
@@ -3019,20 +3133,22 @@
       <c r="N13">
         <v>3</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="P13" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="P13" t="s">
+      <c r="Q13" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" s="19" t="s">
         <v>144</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" s="19"/>
+      <c r="T13" s="19"/>
+      <c r="U13" s="21" t="s">
         <v>145</v>
-      </c>
-      <c r="U13" t="s">
-        <v>146</v>
       </c>
       <c r="AK13">
         <v>1</v>
@@ -3044,27 +3160,34 @@
         <v>51312</v>
       </c>
       <c r="AT13" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AU13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="BC13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK13" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" t="s">
         <v>67</v>
       </c>
       <c r="D14" t="s">
-        <v>149</v>
-      </c>
+        <v>148</v>
+      </c>
+      <c r="F14" s="16"/>
       <c r="J14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L14">
         <v>4</v>
@@ -3072,20 +3195,22 @@
       <c r="N14">
         <v>3</v>
       </c>
-      <c r="O14" t="s">
+      <c r="O14" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="P14" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="P14" t="s">
+      <c r="Q14" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" s="19"/>
+      <c r="T14" s="19"/>
+      <c r="U14" s="21" t="s">
         <v>153</v>
-      </c>
-      <c r="U14" t="s">
-        <v>154</v>
       </c>
       <c r="AK14">
         <v>1</v>
@@ -3097,27 +3222,34 @@
         <v>51312</v>
       </c>
       <c r="AT14" t="s">
+        <v>154</v>
+      </c>
+      <c r="AU14" t="s">
         <v>155</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>156</v>
       </c>
       <c r="BC14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK14" s="21">
+        <v>2</v>
+      </c>
+      <c r="BL14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C15" t="s">
         <v>67</v>
       </c>
       <c r="D15" t="s">
-        <v>158</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="F15" s="16"/>
       <c r="J15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L15">
         <v>4</v>
@@ -3125,20 +3257,22 @@
       <c r="N15">
         <v>3</v>
       </c>
-      <c r="O15" t="s">
+      <c r="O15" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="P15" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="P15" t="s">
+      <c r="Q15" s="19" t="s">
         <v>160</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="R15" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="U15" t="s">
-        <v>154</v>
+      <c r="S15" s="19"/>
+      <c r="T15" s="19"/>
+      <c r="U15" s="21" t="s">
+        <v>153</v>
       </c>
       <c r="AK15">
         <v>1</v>
@@ -3150,30 +3284,36 @@
         <v>51312</v>
       </c>
       <c r="AT15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AU15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="BC15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="BK15" s="21">
+        <v>2</v>
+      </c>
+      <c r="BL15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" t="s">
+        <v>333</v>
+      </c>
+      <c r="D16" t="s">
         <v>164</v>
       </c>
-      <c r="C16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" t="s">
-        <v>165</v>
-      </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="J16" t="s">
         <v>69</v>
-      </c>
-      <c r="J16" t="s">
-        <v>70</v>
       </c>
       <c r="L16">
         <v>4</v>
@@ -3181,20 +3321,22 @@
       <c r="N16">
         <v>3</v>
       </c>
-      <c r="O16" t="s">
+      <c r="O16" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="P16" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="P16" t="s">
+      <c r="Q16" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="R16" t="s">
+      <c r="S16" s="19"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="21" t="s">
         <v>169</v>
-      </c>
-      <c r="U16" t="s">
-        <v>170</v>
       </c>
       <c r="AK16">
         <v>1</v>
@@ -3206,27 +3348,34 @@
         <v>51312</v>
       </c>
       <c r="AT16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AU16" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="BC16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK16" s="21">
+        <v>2</v>
+      </c>
+      <c r="BL16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" t="s">
+        <v>332</v>
+      </c>
+      <c r="D17" t="s">
         <v>171</v>
       </c>
-      <c r="C17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D17" t="s">
-        <v>172</v>
-      </c>
+      <c r="F17" s="16"/>
       <c r="J17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L17">
         <v>4</v>
@@ -3234,20 +3383,22 @@
       <c r="N17">
         <v>3</v>
       </c>
-      <c r="O17" s="17" t="s">
-        <v>319</v>
-      </c>
-      <c r="P17" s="17" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q17" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="R17" s="17" t="s">
-        <v>322</v>
-      </c>
-      <c r="U17" t="s">
-        <v>323</v>
+      <c r="O17" s="19" t="s">
+        <v>344</v>
+      </c>
+      <c r="P17" s="19" t="s">
+        <v>345</v>
+      </c>
+      <c r="Q17" s="19" t="s">
+        <v>346</v>
+      </c>
+      <c r="R17" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="23" t="s">
+        <v>117</v>
       </c>
       <c r="AK17">
         <v>1</v>
@@ -3259,27 +3410,34 @@
         <v>51312</v>
       </c>
       <c r="AT17" t="s">
+        <v>172</v>
+      </c>
+      <c r="AU17" t="s">
         <v>173</v>
-      </c>
-      <c r="AU17" t="s">
-        <v>174</v>
       </c>
       <c r="BC17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK17" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C18" t="s">
         <v>67</v>
       </c>
       <c r="D18" t="s">
-        <v>176</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="F18" s="16"/>
       <c r="J18" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L18">
         <v>4</v>
@@ -3287,20 +3445,22 @@
       <c r="N18">
         <v>3</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O18" s="19" t="s">
+        <v>176</v>
+      </c>
+      <c r="P18" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="P18" t="s">
+      <c r="Q18" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="R18" t="s">
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="21" t="s">
         <v>180</v>
-      </c>
-      <c r="U18" t="s">
-        <v>181</v>
       </c>
       <c r="AK18">
         <v>1</v>
@@ -3312,27 +3472,34 @@
         <v>51312</v>
       </c>
       <c r="AT18" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AU18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="BC18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK18" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>182</v>
+      </c>
+      <c r="C19" t="s">
+        <v>332</v>
+      </c>
+      <c r="D19" t="s">
         <v>183</v>
       </c>
-      <c r="C19" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" t="s">
-        <v>184</v>
-      </c>
+      <c r="F19" s="16"/>
       <c r="J19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L19">
         <v>4</v>
@@ -3340,20 +3507,22 @@
       <c r="N19">
         <v>3</v>
       </c>
-      <c r="O19" s="17" t="s">
-        <v>324</v>
-      </c>
-      <c r="P19" s="17" t="s">
-        <v>325</v>
-      </c>
-      <c r="Q19" s="17" t="s">
-        <v>326</v>
-      </c>
-      <c r="R19" s="17" t="s">
-        <v>327</v>
-      </c>
-      <c r="U19" t="s">
-        <v>118</v>
+      <c r="O19" s="19" t="s">
+        <v>348</v>
+      </c>
+      <c r="P19" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="Q19" s="19" t="s">
+        <v>350</v>
+      </c>
+      <c r="R19" s="19" t="s">
+        <v>351</v>
+      </c>
+      <c r="S19" s="19"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="21" t="s">
+        <v>117</v>
       </c>
       <c r="AK19">
         <v>1</v>
@@ -3365,27 +3534,34 @@
         <v>51312</v>
       </c>
       <c r="AT19" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AU19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="BC19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK19" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C20" t="s">
         <v>67</v>
       </c>
       <c r="D20" t="s">
-        <v>187</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="F20" s="16"/>
       <c r="J20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L20">
         <v>4</v>
@@ -3393,20 +3569,22 @@
       <c r="N20">
         <v>3</v>
       </c>
-      <c r="O20" t="s">
+      <c r="O20" s="19" t="s">
+        <v>187</v>
+      </c>
+      <c r="P20" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="P20" t="s">
+      <c r="Q20" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" s="19" t="s">
         <v>190</v>
       </c>
-      <c r="R20" t="s">
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="21" t="s">
         <v>191</v>
-      </c>
-      <c r="U20" t="s">
-        <v>192</v>
       </c>
       <c r="AK20">
         <v>1</v>
@@ -3418,30 +3596,34 @@
         <v>51312</v>
       </c>
       <c r="AT20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="AU20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="BC20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK20" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C21" t="s">
         <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>195</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>328</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="F21" s="18"/>
       <c r="J21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L21">
         <v>4</v>
@@ -3449,20 +3631,22 @@
       <c r="N21">
         <v>3</v>
       </c>
-      <c r="O21" t="s">
+      <c r="O21" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="P21" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="P21" t="s">
+      <c r="Q21" s="19" t="s">
         <v>197</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" s="19" t="s">
         <v>198</v>
       </c>
-      <c r="R21" t="s">
-        <v>199</v>
-      </c>
-      <c r="U21" t="s">
-        <v>99</v>
+      <c r="S21" s="19"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="AK21">
         <v>1</v>
@@ -3474,30 +3658,34 @@
         <v>51312</v>
       </c>
       <c r="AT21" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU21" t="s">
         <v>200</v>
-      </c>
-      <c r="AU21" t="s">
-        <v>201</v>
       </c>
       <c r="BC21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK21" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C22" t="s">
         <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>203</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>328</v>
-      </c>
+        <v>202</v>
+      </c>
+      <c r="F22" s="18"/>
       <c r="J22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L22">
         <v>4</v>
@@ -3505,20 +3693,22 @@
       <c r="N22">
         <v>3</v>
       </c>
-      <c r="O22" t="s">
+      <c r="O22" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="P22" s="19" t="s">
         <v>204</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" s="19" t="s">
         <v>205</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="R22" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="R22" t="s">
-        <v>207</v>
-      </c>
-      <c r="U22" t="s">
-        <v>154</v>
+      <c r="S22" s="19"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="21" t="s">
+        <v>153</v>
       </c>
       <c r="AK22">
         <v>1</v>
@@ -3530,30 +3720,34 @@
         <v>51312</v>
       </c>
       <c r="AT22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AU22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="BC22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK22" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C23" t="s">
         <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>210</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>328</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="F23" s="18"/>
       <c r="J23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L23">
         <v>4</v>
@@ -3561,20 +3755,22 @@
       <c r="N23">
         <v>3</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O23" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="P23" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="P23" t="s">
+      <c r="Q23" s="19" t="s">
         <v>212</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="R23" s="19" t="s">
         <v>213</v>
       </c>
-      <c r="R23" t="s">
-        <v>214</v>
-      </c>
-      <c r="U23" t="s">
-        <v>133</v>
+      <c r="S23" s="19"/>
+      <c r="T23" s="19"/>
+      <c r="U23" s="21" t="s">
+        <v>132</v>
       </c>
       <c r="AK23">
         <v>1</v>
@@ -3586,30 +3782,36 @@
         <v>51312</v>
       </c>
       <c r="AT23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AU23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="BC23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK23" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>215</v>
+      </c>
+      <c r="C24" t="s">
+        <v>331</v>
+      </c>
+      <c r="D24" t="s">
         <v>216</v>
       </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" t="s">
-        <v>217</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>339</v>
+      <c r="F24" s="17" t="s">
+        <v>322</v>
       </c>
       <c r="J24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L24">
         <v>4</v>
@@ -3617,20 +3819,22 @@
       <c r="N24">
         <v>3</v>
       </c>
-      <c r="O24" t="s">
+      <c r="O24" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="P24" s="19" t="s">
         <v>218</v>
       </c>
-      <c r="P24" t="s">
+      <c r="Q24" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="R24" t="s">
-        <v>221</v>
-      </c>
-      <c r="U24" t="s">
-        <v>118</v>
+      <c r="S24" s="19"/>
+      <c r="T24" s="19"/>
+      <c r="U24" s="21" t="s">
+        <v>117</v>
       </c>
       <c r="AK24">
         <v>1</v>
@@ -3642,30 +3846,36 @@
         <v>51312</v>
       </c>
       <c r="AT24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AU24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="BC24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK24" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>222</v>
+      </c>
+      <c r="C25" t="s">
+        <v>331</v>
+      </c>
+      <c r="D25" t="s">
         <v>223</v>
       </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" t="s">
-        <v>224</v>
-      </c>
       <c r="F25" s="17" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="J25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L25">
         <v>4</v>
@@ -3673,20 +3883,22 @@
       <c r="N25">
         <v>3</v>
       </c>
-      <c r="O25" t="s">
+      <c r="O25" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="P25" s="19" t="s">
         <v>225</v>
       </c>
-      <c r="P25" t="s">
+      <c r="Q25" s="19" t="s">
         <v>226</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="R25" s="19" t="s">
         <v>227</v>
       </c>
-      <c r="R25" t="s">
-        <v>228</v>
-      </c>
-      <c r="U25" t="s">
-        <v>118</v>
+      <c r="S25" s="19"/>
+      <c r="T25" s="19"/>
+      <c r="U25" s="21" t="s">
+        <v>117</v>
       </c>
       <c r="AK25">
         <v>1</v>
@@ -3698,27 +3910,34 @@
         <v>51312</v>
       </c>
       <c r="AT25" t="s">
+        <v>228</v>
+      </c>
+      <c r="AU25" t="s">
         <v>229</v>
-      </c>
-      <c r="AU25" t="s">
-        <v>230</v>
       </c>
       <c r="BC25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK25" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C26" t="s">
         <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>232</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="F26" s="17"/>
       <c r="J26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L26">
         <v>4</v>
@@ -3726,20 +3945,22 @@
       <c r="N26">
         <v>4</v>
       </c>
-      <c r="O26" t="s">
+      <c r="O26" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="P26" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="P26" t="s">
+      <c r="Q26" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="R26" t="s">
+      <c r="S26" s="19"/>
+      <c r="T26" s="19"/>
+      <c r="U26" s="21" t="s">
         <v>236</v>
-      </c>
-      <c r="U26" t="s">
-        <v>237</v>
       </c>
       <c r="AK26">
         <v>1</v>
@@ -3751,30 +3972,36 @@
         <v>51312</v>
       </c>
       <c r="AT26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AU26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="BC26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK26" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>238</v>
+      </c>
+      <c r="C27" t="s">
+        <v>331</v>
+      </c>
+      <c r="D27" t="s">
         <v>239</v>
       </c>
-      <c r="C27" t="s">
-        <v>67</v>
-      </c>
-      <c r="D27" t="s">
-        <v>240</v>
-      </c>
       <c r="F27" s="17" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="J27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L27">
         <v>4</v>
@@ -3782,20 +4009,22 @@
       <c r="N27">
         <v>3</v>
       </c>
-      <c r="O27" t="s">
+      <c r="O27" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="P27" s="19" t="s">
         <v>241</v>
       </c>
-      <c r="P27" t="s">
+      <c r="Q27" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="R27" t="s">
-        <v>244</v>
-      </c>
-      <c r="U27" t="s">
-        <v>133</v>
+      <c r="S27" s="19"/>
+      <c r="T27" s="19"/>
+      <c r="U27" s="21" t="s">
+        <v>132</v>
       </c>
       <c r="AK27">
         <v>1</v>
@@ -3807,30 +4036,34 @@
         <v>51312</v>
       </c>
       <c r="AT27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AU27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="BC27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK27" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C28" t="s">
         <v>67</v>
       </c>
       <c r="D28" t="s">
-        <v>247</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>328</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="F28" s="18"/>
       <c r="J28" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L28">
         <v>4</v>
@@ -3838,20 +4071,22 @@
       <c r="N28">
         <v>3</v>
       </c>
-      <c r="O28" t="s">
+      <c r="O28" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="P28" s="19" t="s">
         <v>248</v>
       </c>
-      <c r="P28" t="s">
+      <c r="Q28" s="19" t="s">
         <v>249</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="R28" s="19" t="s">
         <v>250</v>
       </c>
-      <c r="R28" t="s">
-        <v>251</v>
-      </c>
-      <c r="U28" t="s">
-        <v>154</v>
+      <c r="S28" s="19"/>
+      <c r="T28" s="19"/>
+      <c r="U28" s="21" t="s">
+        <v>153</v>
       </c>
       <c r="AK28">
         <v>1</v>
@@ -3863,30 +4098,34 @@
         <v>51312</v>
       </c>
       <c r="AT28" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AU28" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BC28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="BK28" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:64" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C29" t="s">
         <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>254</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>328</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="F29" s="18"/>
       <c r="J29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L29">
         <v>4</v>
@@ -3894,20 +4133,22 @@
       <c r="N29">
         <v>3</v>
       </c>
-      <c r="O29" t="s">
+      <c r="O29" s="19" t="s">
+        <v>254</v>
+      </c>
+      <c r="P29" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="P29" t="s">
+      <c r="Q29" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="R29" t="s">
-        <v>258</v>
-      </c>
-      <c r="U29" t="s">
-        <v>192</v>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="21" t="s">
+        <v>191</v>
       </c>
       <c r="AK29">
         <v>1</v>
@@ -3919,13 +4160,19 @@
         <v>51312</v>
       </c>
       <c r="AT29" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AU29" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="BC29">
         <v>0</v>
+      </c>
+      <c r="BK29" s="21">
+        <v>3</v>
+      </c>
+      <c r="BL29">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -3944,380 +4191,380 @@
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.77734375" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
-    <col min="3" max="3" width="37.21875" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-    </row>
-    <row r="2" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>262</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="D2" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="F2" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="F2" s="14" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="B3" s="7">
+        <v>4</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="B3" s="8">
+      <c r="D3" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>270</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="D5" s="7"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D6" s="7"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B7" s="8">
         <v>4</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C7" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>268</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>269</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="12" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8" t="s">
-        <v>276</v>
-      </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="B7" s="9">
+      <c r="E7" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B11" s="7">
         <v>4</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="F7" s="7"/>
-      <c r="G7" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" ht="17.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="B11" s="8">
+      <c r="D11" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="B14" s="8">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="D15" s="8"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="B16" s="7">
         <v>4</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" ht="32.549999999999997" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="B14" s="9">
-        <v>3</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>290</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>291</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="B16" s="8">
+      <c r="D16" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="6"/>
+    </row>
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B20" s="8">
         <v>4</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="7"/>
-    </row>
-    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8" t="s">
-        <v>299</v>
-      </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="7"/>
-    </row>
-    <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="B20" s="9">
-        <v>4</v>
-      </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>301</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="E20" s="9" t="s">
+      <c r="F20" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="F20" s="7" t="s">
+    </row>
+    <row r="21" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" ht="22.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:6" ht="23.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="22" spans="1:6" ht="23.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="9" t="s">
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="7"/>
-    </row>
-    <row r="23" spans="1:6" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="9" t="s">
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="7"/>
-    </row>
-    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="B24" s="7">
+        <v>5</v>
+      </c>
+      <c r="C24" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="B24" s="8">
-        <v>5</v>
-      </c>
-      <c r="C24" s="8" t="s">
+      <c r="D24" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="F24" s="6"/>
+    </row>
+    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7" t="s">
         <v>308</v>
       </c>
-      <c r="D24" s="8" t="s">
-        <v>269</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="F24" s="7"/>
-    </row>
-    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="7"/>
-    </row>
-    <row r="26" spans="1:6" ht="20.55" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8" t="s">
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="7"/>
-    </row>
-    <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8" t="s">
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8" t="s">
-        <v>312</v>
-      </c>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="7"/>
-    </row>
-    <row r="29" spans="1:6" ht="13.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:6" ht="16.05" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="6"/>
+    </row>
+    <row r="29" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" display="https://www.biwe-bbq.de/weiterbildungsportal/themen/coaching-qualifizierung/einzelansicht/tq-lagerlogistik" xr:uid="{508EE104-A0F6-4678-8237-1AA62422A333}"/>
@@ -4333,6 +4580,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100879B58D3C23DCA4AAEF47596CA4D8E48" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee8b9d8723b80ccc4cb578ffd4faacc7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02625a54-df84-4a3b-b049-0bb7e92cde0d" xmlns:ns3="c90f9e10-81f0-426e-b8bb-fc89022b3796" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="64b8ed4db9a6e136c161da669116b9cc" ns2:_="" ns3:_="">
     <xsd:import namespace="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
@@ -4541,41 +4808,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="02625a54-df84-4a3b-b049-0bb7e92cde0d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A223085B-57B4-40DB-BC96-92703C914FDC}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
-    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -4598,9 +4834,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A223085B-57B4-40DB-BC96-92703C914FDC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="02625a54-df84-4a3b-b049-0bb7e92cde0d"/>
+    <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed excel error image associaten wrong added image count to questions and answers
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/221111_Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/221111_Booklet_FK_Lagerlogistik.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IvanaBoscolo\source\repos\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B75FF7-A283-4638-A3D2-785B315F0A95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA3F2A6-0A8F-485E-9EDD-C3F5CC33FD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16035" yWindow="8640" windowWidth="32235" windowHeight="21945" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="23100" yWindow="96" windowWidth="23016" windowHeight="25200" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,28 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="474" uniqueCount="357">
   <si>
@@ -1049,9 +1071,6 @@
     <t>SK34A02_Karton_eingerissen.png</t>
   </si>
   <si>
-    <t>SK34B01_Sicherheitshinweis_Schuhe</t>
-  </si>
-  <si>
     <t>SK34B02_Pfuetze_Gabelstapler.png</t>
   </si>
   <si>
@@ -1113,6 +1132,9 @@
   </si>
   <si>
     <t>AmountAnswers</t>
+  </si>
+  <si>
+    <t>SK34B01_Sicherheitshinweis_Schuhe.png</t>
   </si>
 </sst>
 </file>
@@ -1352,7 +1374,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1828,7 +1853,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}" name="Tabelle5" displayName="Tabelle5" ref="A1:BO29" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}" name="Tabelle5" displayName="Tabelle5" ref="A1:BO29" totalsRowShown="0" headerRowDxfId="12" headerRowBorderDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="A1:BO29" xr:uid="{96A82516-1A7E-498A-AF83-1E1CB83B81EF}"/>
   <tableColumns count="67">
     <tableColumn id="1" xr3:uid="{5027A3BA-AE24-48AB-84F1-2B75CE07B771}" name="ItemID"/>
@@ -1897,22 +1922,24 @@
     <tableColumn id="38" xr3:uid="{179223B5-3B0E-4CBE-B1C9-0C2EA9F0C960}" name="CourseId"/>
     <tableColumn id="45" xr3:uid="{75FC8F54-CC63-4DA4-889F-ACD788549AEC}" name="QuestionHasPicture"/>
     <tableColumn id="46" xr3:uid="{1C807CB8-6254-47D5-AE14-42097F7410E0}" name="AnswerHasPicture"/>
-    <tableColumn id="51" xr3:uid="{C8723145-CFAE-43B6-A144-0DC21813B4CD}" name="AmountAnswers"/>
+    <tableColumn id="51" xr3:uid="{C8723145-CFAE-43B6-A144-0DC21813B4CD}" name="AmountAnswers" dataDxfId="0">
+      <calculatedColumnFormula array="1">SUM(--(LEN(TRIM(O2:T2))&gt;0))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FA6BC1E8-B21A-4128-8A22-70A637C907C7}" name="Tabelle2" displayName="Tabelle2" ref="A2:F28" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FA6BC1E8-B21A-4128-8A22-70A637C907C7}" name="Tabelle2" displayName="Tabelle2" ref="A2:F28" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8">
   <autoFilter ref="A2:F28" xr:uid="{32F97D7E-8812-4F9B-8AF1-1B0319C7EBEB}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C51C7E93-CE6E-4C1B-AD58-A874E285D9B0}" name="Kompetenzbereich / TQ /Handlungsfeld" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{F09C954C-5D34-4A50-8E7B-35DC50BC476C}" name="Anzahl der Items pro Handlungsfeld " dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{B85CCA84-7CA3-4504-8C89-704D1754AC42}" name="Handlungssituation" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{DFFF5463-9DA0-41F4-8B1D-D52E4CDF5D17}" name="Mapping " dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{247742C6-96B2-4270-9601-0D0BB349E08F}" name="Matching Biwe TQ" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{7E268660-F79E-407E-A5A7-046099DFE392}" name="Allgemeine Auswertung des Skill Asssessments - Abschlussscreen " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C51C7E93-CE6E-4C1B-AD58-A874E285D9B0}" name="Kompetenzbereich / TQ /Handlungsfeld" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{F09C954C-5D34-4A50-8E7B-35DC50BC476C}" name="Anzahl der Items pro Handlungsfeld " dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{B85CCA84-7CA3-4504-8C89-704D1754AC42}" name="Handlungssituation" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{DFFF5463-9DA0-41F4-8B1D-D52E4CDF5D17}" name="Mapping " dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{247742C6-96B2-4270-9601-0D0BB349E08F}" name="Matching Biwe TQ" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{7E268660-F79E-407E-A5A7-046099DFE392}" name="Allgemeine Auswertung des Skill Asssessments - Abschlussscreen " dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2217,19 +2244,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
   <dimension ref="A1:BO29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
+      <selection activeCell="BN2" sqref="BN2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.42578125" customWidth="1"/>
-    <col min="46" max="46" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.44140625" customWidth="1"/>
+    <col min="46" max="46" width="38.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="39" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:67" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2417,22 +2444,22 @@
         <v>330</v>
       </c>
       <c r="BK1" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="BL1" s="22" t="s">
         <v>352</v>
       </c>
-      <c r="BL1" s="22" t="s">
+      <c r="BM1" s="22" t="s">
         <v>353</v>
       </c>
-      <c r="BM1" s="22" t="s">
+      <c r="BN1" s="22" t="s">
         <v>354</v>
       </c>
-      <c r="BN1" s="22" t="s">
+      <c r="BO1" s="22" t="s">
         <v>355</v>
       </c>
-      <c r="BO1" s="22" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -2493,8 +2520,18 @@
       <c r="BL2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM2">
+        <v>0</v>
+      </c>
+      <c r="BN2">
+        <v>0</v>
+      </c>
+      <c r="BO2" cm="1">
+        <f t="array" ref="BO2">SUM(--(LEN(TRIM(O2:T2))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -2557,8 +2594,18 @@
       <c r="BL3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM3">
+        <v>1</v>
+      </c>
+      <c r="BN3">
+        <v>0</v>
+      </c>
+      <c r="BO3" s="21" cm="1">
+        <f t="array" ref="BO3">SUM(--(LEN(TRIM(O3:T3))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -2619,8 +2666,18 @@
       <c r="BL4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM4">
+        <v>0</v>
+      </c>
+      <c r="BN4">
+        <v>0</v>
+      </c>
+      <c r="BO4" s="21" cm="1">
+        <f t="array" ref="BO4">SUM(--(LEN(TRIM(O4:T4))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -2681,8 +2738,18 @@
       <c r="BL5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM5">
+        <v>0</v>
+      </c>
+      <c r="BN5">
+        <v>0</v>
+      </c>
+      <c r="BO5" s="21" cm="1">
+        <f t="array" ref="BO5">SUM(--(LEN(TRIM(O5:T5))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -2693,7 +2760,7 @@
         <v>93</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>335</v>
+        <v>356</v>
       </c>
       <c r="J6" t="s">
         <v>69</v>
@@ -2745,8 +2812,18 @@
       <c r="BL6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM6">
+        <v>1</v>
+      </c>
+      <c r="BN6">
+        <v>0</v>
+      </c>
+      <c r="BO6" s="21" cm="1">
+        <f t="array" ref="BO6">SUM(--(LEN(TRIM(O6:T6))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>101</v>
       </c>
@@ -2757,7 +2834,7 @@
         <v>102</v>
       </c>
       <c r="F7" s="17" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="J7" t="s">
         <v>69</v>
@@ -2809,8 +2886,18 @@
       <c r="BL7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM7">
+        <v>1</v>
+      </c>
+      <c r="BN7">
+        <v>0</v>
+      </c>
+      <c r="BO7" s="21" cm="1">
+        <f t="array" ref="BO7">SUM(--(LEN(TRIM(O7:T7))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>108</v>
       </c>
@@ -2831,16 +2918,16 @@
         <v>3</v>
       </c>
       <c r="O8" s="20" t="s">
+        <v>339</v>
+      </c>
+      <c r="P8" s="20" t="s">
         <v>340</v>
       </c>
-      <c r="P8" s="20" t="s">
+      <c r="Q8" s="20" t="s">
         <v>341</v>
       </c>
-      <c r="Q8" s="20" t="s">
+      <c r="R8" s="20" t="s">
         <v>342</v>
-      </c>
-      <c r="R8" s="20" t="s">
-        <v>343</v>
       </c>
       <c r="S8" s="19"/>
       <c r="T8" s="19"/>
@@ -2871,8 +2958,18 @@
       <c r="BL8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM8">
+        <v>0</v>
+      </c>
+      <c r="BN8">
+        <v>4</v>
+      </c>
+      <c r="BO8" s="21" cm="1">
+        <f t="array" ref="BO8">SUM(--(LEN(TRIM(O8:T8))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>111</v>
       </c>
@@ -2883,7 +2980,7 @@
         <v>112</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="J9" t="s">
         <v>69</v>
@@ -2935,8 +3032,18 @@
       <c r="BL9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM9">
+        <v>1</v>
+      </c>
+      <c r="BN9">
+        <v>0</v>
+      </c>
+      <c r="BO9" s="21" cm="1">
+        <f t="array" ref="BO9">SUM(--(LEN(TRIM(O9:T9))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>119</v>
       </c>
@@ -3009,8 +3116,18 @@
       <c r="BL10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM10">
+        <v>0</v>
+      </c>
+      <c r="BN10">
+        <v>4</v>
+      </c>
+      <c r="BO10" s="21" cm="1">
+        <f t="array" ref="BO10">SUM(--(LEN(TRIM(O10:T10))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -3071,8 +3188,18 @@
       <c r="BL11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM11">
+        <v>0</v>
+      </c>
+      <c r="BN11">
+        <v>0</v>
+      </c>
+      <c r="BO11" s="21" cm="1">
+        <f t="array" ref="BO11">SUM(--(LEN(TRIM(O11:T11))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>133</v>
       </c>
@@ -3083,7 +3210,7 @@
         <v>134</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J12" t="s">
         <v>69</v>
@@ -3133,8 +3260,18 @@
       <c r="BL12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM12">
+        <v>1</v>
+      </c>
+      <c r="BN12">
+        <v>0</v>
+      </c>
+      <c r="BO12" s="21" cm="1">
+        <f t="array" ref="BO12">SUM(--(LEN(TRIM(O12:T12))&gt;0))</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>139</v>
       </c>
@@ -3195,8 +3332,18 @@
       <c r="BL13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM13">
+        <v>0</v>
+      </c>
+      <c r="BN13">
+        <v>0</v>
+      </c>
+      <c r="BO13" s="21" cm="1">
+        <f t="array" ref="BO13">SUM(--(LEN(TRIM(O13:T13))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>147</v>
       </c>
@@ -3257,8 +3404,18 @@
       <c r="BL14">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM14">
+        <v>0</v>
+      </c>
+      <c r="BN14">
+        <v>0</v>
+      </c>
+      <c r="BO14" s="21" cm="1">
+        <f t="array" ref="BO14">SUM(--(LEN(TRIM(O14:T14))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>156</v>
       </c>
@@ -3319,8 +3476,18 @@
       <c r="BL15">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.2">
+      <c r="BM15">
+        <v>0</v>
+      </c>
+      <c r="BN15">
+        <v>0</v>
+      </c>
+      <c r="BO15" s="21" cm="1">
+        <f t="array" ref="BO15">SUM(--(LEN(TRIM(O15:T15))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>163</v>
       </c>
@@ -3331,7 +3498,7 @@
         <v>164</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="J16" t="s">
         <v>69</v>
@@ -3383,8 +3550,18 @@
       <c r="BL16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM16">
+        <v>1</v>
+      </c>
+      <c r="BN16">
+        <v>0</v>
+      </c>
+      <c r="BO16" s="21" cm="1">
+        <f t="array" ref="BO16">SUM(--(LEN(TRIM(O16:T16))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>170</v>
       </c>
@@ -3405,16 +3582,16 @@
         <v>3</v>
       </c>
       <c r="O17" s="19" t="s">
+        <v>343</v>
+      </c>
+      <c r="P17" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="P17" s="19" t="s">
+      <c r="Q17" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="Q17" s="19" t="s">
+      <c r="R17" s="19" t="s">
         <v>346</v>
-      </c>
-      <c r="R17" s="19" t="s">
-        <v>347</v>
       </c>
       <c r="S17" s="19"/>
       <c r="T17" s="19"/>
@@ -3445,8 +3622,18 @@
       <c r="BL17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM17">
+        <v>0</v>
+      </c>
+      <c r="BN17">
+        <v>4</v>
+      </c>
+      <c r="BO17" s="21" cm="1">
+        <f t="array" ref="BO17">SUM(--(LEN(TRIM(O17:T17))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>174</v>
       </c>
@@ -3507,8 +3694,18 @@
       <c r="BL18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM18">
+        <v>0</v>
+      </c>
+      <c r="BN18">
+        <v>0</v>
+      </c>
+      <c r="BO18" s="21" cm="1">
+        <f t="array" ref="BO18">SUM(--(LEN(TRIM(O18:T18))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>182</v>
       </c>
@@ -3529,16 +3726,16 @@
         <v>3</v>
       </c>
       <c r="O19" s="19" t="s">
+        <v>347</v>
+      </c>
+      <c r="P19" s="19" t="s">
         <v>348</v>
       </c>
-      <c r="P19" s="19" t="s">
+      <c r="Q19" s="19" t="s">
         <v>349</v>
       </c>
-      <c r="Q19" s="19" t="s">
+      <c r="R19" s="19" t="s">
         <v>350</v>
-      </c>
-      <c r="R19" s="19" t="s">
-        <v>351</v>
       </c>
       <c r="S19" s="19"/>
       <c r="T19" s="19"/>
@@ -3569,8 +3766,18 @@
       <c r="BL19">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM19">
+        <v>0</v>
+      </c>
+      <c r="BN19">
+        <v>4</v>
+      </c>
+      <c r="BO19" s="21" cm="1">
+        <f t="array" ref="BO19">SUM(--(LEN(TRIM(O19:T19))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>185</v>
       </c>
@@ -3631,8 +3838,18 @@
       <c r="BL20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM20">
+        <v>0</v>
+      </c>
+      <c r="BN20">
+        <v>0</v>
+      </c>
+      <c r="BO20" s="21" cm="1">
+        <f t="array" ref="BO20">SUM(--(LEN(TRIM(O20:T20))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>193</v>
       </c>
@@ -3693,8 +3910,18 @@
       <c r="BL21">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM21">
+        <v>0</v>
+      </c>
+      <c r="BN21">
+        <v>0</v>
+      </c>
+      <c r="BO21" s="21" cm="1">
+        <f t="array" ref="BO21">SUM(--(LEN(TRIM(O21:T21))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>201</v>
       </c>
@@ -3755,8 +3982,18 @@
       <c r="BL22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM22">
+        <v>0</v>
+      </c>
+      <c r="BN22">
+        <v>0</v>
+      </c>
+      <c r="BO22" s="21" cm="1">
+        <f t="array" ref="BO22">SUM(--(LEN(TRIM(O22:T22))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>208</v>
       </c>
@@ -3817,8 +4054,18 @@
       <c r="BL23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM23">
+        <v>0</v>
+      </c>
+      <c r="BN23">
+        <v>0</v>
+      </c>
+      <c r="BO23" s="21" cm="1">
+        <f t="array" ref="BO23">SUM(--(LEN(TRIM(O23:T23))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>215</v>
       </c>
@@ -3881,8 +4128,18 @@
       <c r="BL24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM24">
+        <v>1</v>
+      </c>
+      <c r="BN24">
+        <v>0</v>
+      </c>
+      <c r="BO24" s="21" cm="1">
+        <f t="array" ref="BO24">SUM(--(LEN(TRIM(O24:T24))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>222</v>
       </c>
@@ -3945,8 +4202,18 @@
       <c r="BL25">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM25">
+        <v>1</v>
+      </c>
+      <c r="BN25">
+        <v>0</v>
+      </c>
+      <c r="BO25" s="21" cm="1">
+        <f t="array" ref="BO25">SUM(--(LEN(TRIM(O25:T25))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>230</v>
       </c>
@@ -4007,8 +4274,18 @@
       <c r="BL26">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM26">
+        <v>0</v>
+      </c>
+      <c r="BN26">
+        <v>0</v>
+      </c>
+      <c r="BO26" s="21" cm="1">
+        <f t="array" ref="BO26">SUM(--(LEN(TRIM(O26:T26))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>238</v>
       </c>
@@ -4071,8 +4348,18 @@
       <c r="BL27">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM27">
+        <v>1</v>
+      </c>
+      <c r="BN27">
+        <v>0</v>
+      </c>
+      <c r="BO27" s="21" cm="1">
+        <f t="array" ref="BO27">SUM(--(LEN(TRIM(O27:T27))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>245</v>
       </c>
@@ -4133,8 +4420,18 @@
       <c r="BL28">
         <v>6</v>
       </c>
-    </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.2">
+      <c r="BM28">
+        <v>0</v>
+      </c>
+      <c r="BN28">
+        <v>0</v>
+      </c>
+      <c r="BO28" s="21" cm="1">
+        <f t="array" ref="BO28">SUM(--(LEN(TRIM(O28:T28))&gt;0))</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:67" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>252</v>
       </c>
@@ -4194,6 +4491,16 @@
       </c>
       <c r="BL29">
         <v>6</v>
+      </c>
+      <c r="BM29">
+        <v>0</v>
+      </c>
+      <c r="BN29">
+        <v>0</v>
+      </c>
+      <c r="BO29" s="21" cm="1">
+        <f t="array" ref="BO29">SUM(--(LEN(TRIM(O29:T29))&gt;0))</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -4215,24 +4522,24 @@
       <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1"/>
-    <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="3" max="3" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>259</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>260</v>
       </c>
@@ -4252,7 +4559,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>266</v>
       </c>
@@ -4275,7 +4582,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7" t="s">
@@ -4288,7 +4595,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7" t="s">
@@ -4298,7 +4605,7 @@
       <c r="E5" s="10"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7" t="s">
@@ -4308,7 +4615,7 @@
       <c r="E6" s="10"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>276</v>
       </c>
@@ -4329,7 +4636,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8" t="s">
@@ -4339,7 +4646,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8" t="s">
@@ -4349,7 +4656,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8" t="s">
@@ -4359,7 +4666,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="17.649999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="17.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>283</v>
       </c>
@@ -4377,7 +4684,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7" t="s">
@@ -4387,7 +4694,7 @@
       <c r="E12" s="7"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7" t="s">
@@ -4397,7 +4704,7 @@
       <c r="E13" s="7"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="32.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>288</v>
       </c>
@@ -4415,7 +4722,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8"/>
       <c r="C15" s="8" t="s">
@@ -4425,7 +4732,7 @@
       <c r="E15" s="9"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:7" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>293</v>
       </c>
@@ -4443,7 +4750,7 @@
       </c>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7" t="s">
@@ -4453,7 +4760,7 @@
       <c r="E17" s="7"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7" t="s">
@@ -4463,7 +4770,7 @@
       <c r="E18" s="7"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7" t="s">
@@ -4473,7 +4780,7 @@
       <c r="E19" s="7"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>299</v>
       </c>
@@ -4493,7 +4800,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="22.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8" t="s">
@@ -4503,7 +4810,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="23.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="23.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="8"/>
       <c r="C22" s="8" t="s">
@@ -4513,7 +4820,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="8" t="s">
@@ -4523,7 +4830,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>306</v>
       </c>
@@ -4541,7 +4848,7 @@
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
@@ -4551,7 +4858,7 @@
       <c r="E25" s="7"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" ht="20.65" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="20.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
@@ -4561,7 +4868,7 @@
       <c r="E26" s="7"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
@@ -4571,7 +4878,7 @@
       <c r="E27" s="7"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
@@ -4581,11 +4888,11 @@
       <c r="E28" s="7"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" ht="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:6" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" display="https://www.biwe-bbq.de/weiterbildungsportal/themen/coaching-qualifizierung/einzelansicht/tq-lagerlogistik" xr:uid="{508EE104-A0F6-4678-8237-1AA62422A333}"/>
@@ -4601,15 +4908,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
@@ -4618,6 +4916,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4830,14 +5137,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -4850,6 +5149,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
added question and answer create
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/221111_Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/221111_Booklet_FK_Lagerlogistik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA3F2A6-0A8F-485E-9EDD-C3F5CC33FD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213FA6F8-9C51-4DB2-9EE6-D93144BABF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23100" yWindow="96" windowWidth="23016" windowHeight="25200" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="19920" yWindow="6876" windowWidth="23016" windowHeight="11580" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -1210,7 +1210,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1241,8 +1241,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="6" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1313,12 +1319,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="6"/>
+      </left>
+      <right style="thin">
+        <color theme="6"/>
+      </right>
+      <top style="thin">
+        <color theme="6"/>
+      </top>
+      <bottom style="thin">
+        <color theme="6"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1369,15 +1390,13 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="13">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1708,6 +1727,9 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="8"/>
@@ -1922,7 +1944,7 @@
     <tableColumn id="38" xr3:uid="{179223B5-3B0E-4CBE-B1C9-0C2EA9F0C960}" name="CourseId"/>
     <tableColumn id="45" xr3:uid="{75FC8F54-CC63-4DA4-889F-ACD788549AEC}" name="QuestionHasPicture"/>
     <tableColumn id="46" xr3:uid="{1C807CB8-6254-47D5-AE14-42097F7410E0}" name="AnswerHasPicture"/>
-    <tableColumn id="51" xr3:uid="{C8723145-CFAE-43B6-A144-0DC21813B4CD}" name="AmountAnswers" dataDxfId="0">
+    <tableColumn id="51" xr3:uid="{C8723145-CFAE-43B6-A144-0DC21813B4CD}" name="AmountAnswers" dataDxfId="9">
       <calculatedColumnFormula array="1">SUM(--(LEN(TRIM(O2:T2))&gt;0))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1931,15 +1953,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FA6BC1E8-B21A-4128-8A22-70A637C907C7}" name="Tabelle2" displayName="Tabelle2" ref="A2:F28" totalsRowShown="0" headerRowDxfId="9" dataDxfId="7" headerRowBorderDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FA6BC1E8-B21A-4128-8A22-70A637C907C7}" name="Tabelle2" displayName="Tabelle2" ref="A2:F28" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7">
   <autoFilter ref="A2:F28" xr:uid="{32F97D7E-8812-4F9B-8AF1-1B0319C7EBEB}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C51C7E93-CE6E-4C1B-AD58-A874E285D9B0}" name="Kompetenzbereich / TQ /Handlungsfeld" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{F09C954C-5D34-4A50-8E7B-35DC50BC476C}" name="Anzahl der Items pro Handlungsfeld " dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{B85CCA84-7CA3-4504-8C89-704D1754AC42}" name="Handlungssituation" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{DFFF5463-9DA0-41F4-8B1D-D52E4CDF5D17}" name="Mapping " dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{247742C6-96B2-4270-9601-0D0BB349E08F}" name="Matching Biwe TQ" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{7E268660-F79E-407E-A5A7-046099DFE392}" name="Allgemeine Auswertung des Skill Asssessments - Abschlussscreen " dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{C51C7E93-CE6E-4C1B-AD58-A874E285D9B0}" name="Kompetenzbereich / TQ /Handlungsfeld" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{F09C954C-5D34-4A50-8E7B-35DC50BC476C}" name="Anzahl der Items pro Handlungsfeld " dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{B85CCA84-7CA3-4504-8C89-704D1754AC42}" name="Handlungssituation" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{DFFF5463-9DA0-41F4-8B1D-D52E4CDF5D17}" name="Mapping " dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{247742C6-96B2-4270-9601-0D0BB349E08F}" name="Matching Biwe TQ" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{7E268660-F79E-407E-A5A7-046099DFE392}" name="Allgemeine Auswertung des Skill Asssessments - Abschlussscreen " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2244,8 +2266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
   <dimension ref="A1:BO29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AT1" workbookViewId="0">
-      <selection activeCell="BN2" sqref="BN2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3063,34 +3085,34 @@
       <c r="N10">
         <v>4</v>
       </c>
-      <c r="O10" s="19" t="s">
-        <v>316</v>
-      </c>
-      <c r="P10" s="19" t="s">
-        <v>317</v>
-      </c>
-      <c r="Q10" s="19" t="s">
-        <v>318</v>
-      </c>
-      <c r="R10" s="19" t="s">
-        <v>319</v>
+      <c r="O10" t="s">
+        <v>124</v>
+      </c>
+      <c r="P10" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>126</v>
+      </c>
+      <c r="R10" t="s">
+        <v>127</v>
       </c>
       <c r="S10" s="19"/>
       <c r="T10" s="19"/>
       <c r="U10" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="AA10" t="s">
-        <v>124</v>
-      </c>
-      <c r="AB10" t="s">
-        <v>125</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>126</v>
-      </c>
-      <c r="AD10" t="s">
-        <v>127</v>
+      <c r="AA10" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="AB10" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="AC10" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="AD10" s="24" t="s">
+        <v>319</v>
       </c>
       <c r="AK10">
         <v>1</v>
@@ -4890,9 +4912,9 @@
     </row>
     <row r="29" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="27" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G3" r:id="rId1" display="https://www.biwe-bbq.de/weiterbildungsportal/themen/coaching-qualifizierung/einzelansicht/tq-lagerlogistik" xr:uid="{508EE104-A0F6-4678-8237-1AA62422A333}"/>
@@ -4908,6 +4930,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
@@ -4916,15 +4947,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5137,6 +5159,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -5149,14 +5179,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
fixed question result vector fixed dbinitializer io exception
</commit_message>
<xml_diff>
--- a/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/221111_Booklet_FK_Lagerlogistik.xlsx
+++ b/src/cloud/backend/apollo.cloud/Graph.Apollo.Cloud.Assessment/Data/221111_Booklet_FK_Lagerlogistik.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PatricBoscolo\source\gh\APOLLO\src\cloud\backend\apollo.cloud\Graph.Apollo.Cloud.Assessment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213FA6F8-9C51-4DB2-9EE6-D93144BABF7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1514529D-6972-456B-B603-53FE860E9EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19920" yWindow="6876" windowWidth="23016" windowHeight="11580" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
+    <workbookView xWindow="-60" yWindow="4008" windowWidth="23016" windowHeight="11580" xr2:uid="{964963E8-EE09-4957-A004-AE51DD5268F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Booklet_FK Lagerlogistik" sheetId="1" r:id="rId1"/>
@@ -34,28 +34,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1944,9 +1922,7 @@
     <tableColumn id="38" xr3:uid="{179223B5-3B0E-4CBE-B1C9-0C2EA9F0C960}" name="CourseId"/>
     <tableColumn id="45" xr3:uid="{75FC8F54-CC63-4DA4-889F-ACD788549AEC}" name="QuestionHasPicture"/>
     <tableColumn id="46" xr3:uid="{1C807CB8-6254-47D5-AE14-42097F7410E0}" name="AnswerHasPicture"/>
-    <tableColumn id="51" xr3:uid="{C8723145-CFAE-43B6-A144-0DC21813B4CD}" name="AmountAnswers" dataDxfId="9">
-      <calculatedColumnFormula array="1">SUM(--(LEN(TRIM(O2:T2))&gt;0))</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="51" xr3:uid="{C8723145-CFAE-43B6-A144-0DC21813B4CD}" name="AmountAnswers" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2266,8 +2242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4694E0-AE11-4213-9084-7EF5B5E33E57}">
   <dimension ref="A1:BO29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+      <selection activeCell="BP1" sqref="BP1:BP1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2548,8 +2524,7 @@
       <c r="BN2">
         <v>0</v>
       </c>
-      <c r="BO2" cm="1">
-        <f t="array" ref="BO2">SUM(--(LEN(TRIM(O2:T2))&gt;0))</f>
+      <c r="BO2" s="21">
         <v>4</v>
       </c>
     </row>
@@ -2622,8 +2597,7 @@
       <c r="BN3">
         <v>0</v>
       </c>
-      <c r="BO3" s="21" cm="1">
-        <f t="array" ref="BO3">SUM(--(LEN(TRIM(O3:T3))&gt;0))</f>
+      <c r="BO3" s="21">
         <v>4</v>
       </c>
     </row>
@@ -2694,8 +2668,7 @@
       <c r="BN4">
         <v>0</v>
       </c>
-      <c r="BO4" s="21" cm="1">
-        <f t="array" ref="BO4">SUM(--(LEN(TRIM(O4:T4))&gt;0))</f>
+      <c r="BO4" s="21">
         <v>4</v>
       </c>
     </row>
@@ -2766,8 +2739,7 @@
       <c r="BN5">
         <v>0</v>
       </c>
-      <c r="BO5" s="21" cm="1">
-        <f t="array" ref="BO5">SUM(--(LEN(TRIM(O5:T5))&gt;0))</f>
+      <c r="BO5" s="21">
         <v>4</v>
       </c>
     </row>
@@ -2840,8 +2812,7 @@
       <c r="BN6">
         <v>0</v>
       </c>
-      <c r="BO6" s="21" cm="1">
-        <f t="array" ref="BO6">SUM(--(LEN(TRIM(O6:T6))&gt;0))</f>
+      <c r="BO6" s="21">
         <v>4</v>
       </c>
     </row>
@@ -2914,8 +2885,7 @@
       <c r="BN7">
         <v>0</v>
       </c>
-      <c r="BO7" s="21" cm="1">
-        <f t="array" ref="BO7">SUM(--(LEN(TRIM(O7:T7))&gt;0))</f>
+      <c r="BO7" s="21">
         <v>4</v>
       </c>
     </row>
@@ -2986,8 +2956,7 @@
       <c r="BN8">
         <v>4</v>
       </c>
-      <c r="BO8" s="21" cm="1">
-        <f t="array" ref="BO8">SUM(--(LEN(TRIM(O8:T8))&gt;0))</f>
+      <c r="BO8" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3060,8 +3029,7 @@
       <c r="BN9">
         <v>0</v>
       </c>
-      <c r="BO9" s="21" cm="1">
-        <f t="array" ref="BO9">SUM(--(LEN(TRIM(O9:T9))&gt;0))</f>
+      <c r="BO9" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3144,8 +3112,7 @@
       <c r="BN10">
         <v>4</v>
       </c>
-      <c r="BO10" s="21" cm="1">
-        <f t="array" ref="BO10">SUM(--(LEN(TRIM(O10:T10))&gt;0))</f>
+      <c r="BO10" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3216,8 +3183,7 @@
       <c r="BN11">
         <v>0</v>
       </c>
-      <c r="BO11" s="21" cm="1">
-        <f t="array" ref="BO11">SUM(--(LEN(TRIM(O11:T11))&gt;0))</f>
+      <c r="BO11" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3288,8 +3254,7 @@
       <c r="BN12">
         <v>0</v>
       </c>
-      <c r="BO12" s="21" cm="1">
-        <f t="array" ref="BO12">SUM(--(LEN(TRIM(O12:T12))&gt;0))</f>
+      <c r="BO12" s="21">
         <v>3</v>
       </c>
     </row>
@@ -3360,8 +3325,7 @@
       <c r="BN13">
         <v>0</v>
       </c>
-      <c r="BO13" s="21" cm="1">
-        <f t="array" ref="BO13">SUM(--(LEN(TRIM(O13:T13))&gt;0))</f>
+      <c r="BO13" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3432,8 +3396,7 @@
       <c r="BN14">
         <v>0</v>
       </c>
-      <c r="BO14" s="21" cm="1">
-        <f t="array" ref="BO14">SUM(--(LEN(TRIM(O14:T14))&gt;0))</f>
+      <c r="BO14" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3504,8 +3467,7 @@
       <c r="BN15">
         <v>0</v>
       </c>
-      <c r="BO15" s="21" cm="1">
-        <f t="array" ref="BO15">SUM(--(LEN(TRIM(O15:T15))&gt;0))</f>
+      <c r="BO15" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3578,8 +3540,7 @@
       <c r="BN16">
         <v>0</v>
       </c>
-      <c r="BO16" s="21" cm="1">
-        <f t="array" ref="BO16">SUM(--(LEN(TRIM(O16:T16))&gt;0))</f>
+      <c r="BO16" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3650,8 +3611,7 @@
       <c r="BN17">
         <v>4</v>
       </c>
-      <c r="BO17" s="21" cm="1">
-        <f t="array" ref="BO17">SUM(--(LEN(TRIM(O17:T17))&gt;0))</f>
+      <c r="BO17" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3722,8 +3682,7 @@
       <c r="BN18">
         <v>0</v>
       </c>
-      <c r="BO18" s="21" cm="1">
-        <f t="array" ref="BO18">SUM(--(LEN(TRIM(O18:T18))&gt;0))</f>
+      <c r="BO18" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3794,8 +3753,7 @@
       <c r="BN19">
         <v>4</v>
       </c>
-      <c r="BO19" s="21" cm="1">
-        <f t="array" ref="BO19">SUM(--(LEN(TRIM(O19:T19))&gt;0))</f>
+      <c r="BO19" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3866,8 +3824,7 @@
       <c r="BN20">
         <v>0</v>
       </c>
-      <c r="BO20" s="21" cm="1">
-        <f t="array" ref="BO20">SUM(--(LEN(TRIM(O20:T20))&gt;0))</f>
+      <c r="BO20" s="21">
         <v>4</v>
       </c>
     </row>
@@ -3938,8 +3895,7 @@
       <c r="BN21">
         <v>0</v>
       </c>
-      <c r="BO21" s="21" cm="1">
-        <f t="array" ref="BO21">SUM(--(LEN(TRIM(O21:T21))&gt;0))</f>
+      <c r="BO21" s="21">
         <v>4</v>
       </c>
     </row>
@@ -4010,8 +3966,7 @@
       <c r="BN22">
         <v>0</v>
       </c>
-      <c r="BO22" s="21" cm="1">
-        <f t="array" ref="BO22">SUM(--(LEN(TRIM(O22:T22))&gt;0))</f>
+      <c r="BO22" s="21">
         <v>4</v>
       </c>
     </row>
@@ -4082,8 +4037,7 @@
       <c r="BN23">
         <v>0</v>
       </c>
-      <c r="BO23" s="21" cm="1">
-        <f t="array" ref="BO23">SUM(--(LEN(TRIM(O23:T23))&gt;0))</f>
+      <c r="BO23" s="21">
         <v>4</v>
       </c>
     </row>
@@ -4156,8 +4110,7 @@
       <c r="BN24">
         <v>0</v>
       </c>
-      <c r="BO24" s="21" cm="1">
-        <f t="array" ref="BO24">SUM(--(LEN(TRIM(O24:T24))&gt;0))</f>
+      <c r="BO24" s="21">
         <v>4</v>
       </c>
     </row>
@@ -4230,8 +4183,7 @@
       <c r="BN25">
         <v>0</v>
       </c>
-      <c r="BO25" s="21" cm="1">
-        <f t="array" ref="BO25">SUM(--(LEN(TRIM(O25:T25))&gt;0))</f>
+      <c r="BO25" s="21">
         <v>4</v>
       </c>
     </row>
@@ -4302,8 +4254,7 @@
       <c r="BN26">
         <v>0</v>
       </c>
-      <c r="BO26" s="21" cm="1">
-        <f t="array" ref="BO26">SUM(--(LEN(TRIM(O26:T26))&gt;0))</f>
+      <c r="BO26" s="21">
         <v>4</v>
       </c>
     </row>
@@ -4376,8 +4327,7 @@
       <c r="BN27">
         <v>0</v>
       </c>
-      <c r="BO27" s="21" cm="1">
-        <f t="array" ref="BO27">SUM(--(LEN(TRIM(O27:T27))&gt;0))</f>
+      <c r="BO27" s="21">
         <v>4</v>
       </c>
     </row>
@@ -4448,8 +4398,7 @@
       <c r="BN28">
         <v>0</v>
       </c>
-      <c r="BO28" s="21" cm="1">
-        <f t="array" ref="BO28">SUM(--(LEN(TRIM(O28:T28))&gt;0))</f>
+      <c r="BO28" s="21">
         <v>4</v>
       </c>
     </row>
@@ -4520,8 +4469,7 @@
       <c r="BN29">
         <v>0</v>
       </c>
-      <c r="BO29" s="21" cm="1">
-        <f t="array" ref="BO29">SUM(--(LEN(TRIM(O29:T29))&gt;0))</f>
+      <c r="BO29" s="21">
         <v>4</v>
       </c>
     </row>
@@ -4930,15 +4878,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="c90f9e10-81f0-426e-b8bb-fc89022b3796" xsi:nil="true"/>
@@ -4947,6 +4886,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5159,14 +5107,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3B3ABF6-4080-46CB-8A76-0A61A3F40BD1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -5179,6 +5119,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="c90f9e10-81f0-426e-b8bb-fc89022b3796"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C63F3413-8325-4072-95D6-266A70C668BD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>